<commit_message>
Teste para manipular campo Time Picker Completo
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="datePicker" sheetId="1" r:id="rId1"/>
+    <sheet name="setup" sheetId="3" r:id="rId1"/>
+    <sheet name="datePicker" sheetId="1" r:id="rId2"/>
+    <sheet name="timePicker" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -42,6 +44,237 @@
   </si>
   <si>
     <t>21/01/1990</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>minuto</t>
+  </si>
+  <si>
+    <t>AmPm</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>Minutos</t>
+  </si>
+  <si>
+    <t>AM_PM</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>34</t>
   </si>
 </sst>
 </file>
@@ -57,15 +290,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -73,13 +312,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,10 +633,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,4 +1043,90 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>setup!$A$4:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>setup!$B$4:$B$63</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>setup!$C$4:$C$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>